<commit_message>
First agentic AI function successful
</commit_message>
<xml_diff>
--- a/pdfs/order_inventory.xlsx
+++ b/pdfs/order_inventory.xlsx
@@ -1,44 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric - Dev\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B85F5AB-9D89-4B4B-B1E1-66FB94DE30DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{E5C539F6-83E3-4722-81CA-0A0782480CD3}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Order Number</t>
   </si>
   <si>
+    <t>Part Number</t>
+  </si>
+  <si>
     <t>Order Details</t>
   </si>
   <si>
@@ -51,7 +34,10 @@
     <t>Buyer</t>
   </si>
   <si>
-    <t>Part Number</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>349584398539</t>
   </si>
   <si>
     <t>2025 HP Laptop</t>
@@ -66,6 +52,12 @@
     <t>Dinasaur Pool Toy</t>
   </si>
   <si>
+    <t>GoPro</t>
+  </si>
+  <si>
+    <t>$100</t>
+  </si>
+  <si>
     <t>Adam</t>
   </si>
   <si>
@@ -78,6 +70,9 @@
     <t>Donna</t>
   </si>
   <si>
+    <t>Brian</t>
+  </si>
+  <si>
     <t>Aaron</t>
   </si>
   <si>
@@ -88,17 +83,25 @@
   </si>
   <si>
     <t>Dorian</t>
+  </si>
+  <si>
+    <t>Tom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,12 +117,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -128,21 +146,15 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -157,44 +169,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -221,32 +233,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -273,24 +267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -302,180 +278,198 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098422C4-0931-4FE6-9000-80F8BD599FBC}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -483,19 +477,19 @@
         <v>23498345933</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2">
         <v>600</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -503,19 +497,19 @@
         <v>23942039482</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1">
+        <v>9</v>
+      </c>
+      <c r="D3">
         <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -523,19 +517,19 @@
         <v>29384023948</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4">
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -543,16 +537,36 @@
         <v>23029849023</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1">
+        <v>11</v>
+      </c>
+      <c r="D5">
         <v>25</v>
       </c>
       <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed homepage background color
</commit_message>
<xml_diff>
--- a/pdfs/order_inventory.xlsx
+++ b/pdfs/order_inventory.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric - Dev\Documents\ai-agent-dev\pdfs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A704F4-C5F8-4CBF-B76E-5E26CEDACBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-750" yWindow="-12675" windowWidth="11475" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -91,8 +97,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,13 +161,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,7 +213,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -233,6 +247,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -267,9 +282,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -442,14 +458,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -489,7 +508,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -509,7 +528,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -529,7 +548,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -549,7 +568,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
fixed RAG excel agent
</commit_message>
<xml_diff>
--- a/pdfs/order_inventory.xlsx
+++ b/pdfs/order_inventory.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric - Dev\Documents\ai-agent-dev\pdfs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A704F4-C5F8-4CBF-B76E-5E26CEDACBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-750" yWindow="-12675" windowWidth="11475" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Order Number</t>
   </si>
@@ -40,10 +34,10 @@
     <t>Buyer</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>349584398539</t>
+    <t>8</t>
+  </si>
+  <si>
+    <t>33945803930</t>
   </si>
   <si>
     <t>2025 HP Laptop</t>
@@ -61,9 +55,18 @@
     <t>GoPro</t>
   </si>
   <si>
+    <t>inflatable boat</t>
+  </si>
+  <si>
+    <t>stuffed animal bunny</t>
+  </si>
+  <si>
     <t>$100</t>
   </si>
   <si>
+    <t>$25</t>
+  </si>
+  <si>
     <t>Adam</t>
   </si>
   <si>
@@ -79,6 +82,12 @@
     <t>Brian</t>
   </si>
   <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
     <t>Aaron</t>
   </si>
   <si>
@@ -92,13 +101,16 @@
   </si>
   <si>
     <t>Tom</t>
+  </si>
+  <si>
+    <t>Felicia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,21 +173,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,7 +217,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -247,7 +251,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -282,10 +285,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -458,17 +460,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -502,13 +501,13 @@
         <v>600</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -522,13 +521,13 @@
         <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -542,13 +541,13 @@
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -562,30 +561,70 @@
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>349584398539</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1290138230948</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D7">
+        <v>500</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed rag excel again
</commit_message>
<xml_diff>
--- a/pdfs/order_inventory.xlsx
+++ b/pdfs/order_inventory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Order Number</t>
   </si>
@@ -34,12 +34,54 @@
     <t>Buyer</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>23498345933</t>
+  </si>
+  <si>
+    <t>23942039482</t>
+  </si>
+  <si>
+    <t>29384023948</t>
+  </si>
+  <si>
+    <t>23029849023</t>
+  </si>
+  <si>
+    <t>349584398539</t>
+  </si>
+  <si>
+    <t>1290138230948</t>
+  </si>
+  <si>
     <t>33945803930</t>
   </si>
   <si>
+    <t>230924802</t>
+  </si>
+  <si>
     <t>2025 HP Laptop</t>
   </si>
   <si>
@@ -61,12 +103,33 @@
     <t>stuffed animal bunny</t>
   </si>
   <si>
+    <t>cactus</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
     <t>$100</t>
   </si>
   <si>
+    <t>500</t>
+  </si>
+  <si>
     <t>$25</t>
   </si>
   <si>
+    <t>$300</t>
+  </si>
+  <si>
     <t>Adam</t>
   </si>
   <si>
@@ -88,6 +151,9 @@
     <t>Kelly</t>
   </si>
   <si>
+    <t>Tim</t>
+  </si>
+  <si>
     <t>Aaron</t>
   </si>
   <si>
@@ -104,6 +170,9 @@
   </si>
   <si>
     <t>Felicia</t>
+  </si>
+  <si>
+    <t>Mike</t>
   </si>
 </sst>
 </file>
@@ -461,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -488,143 +557,163 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>23498345933</v>
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>600</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>23942039482</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
         <v>50</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>29384023948</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>23029849023</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>349584398539</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>1290138230948</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>500</v>
+      <c r="D7" t="s">
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working for first request not second
</commit_message>
<xml_diff>
--- a/pdfs/order_inventory.xlsx
+++ b/pdfs/order_inventory.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric - Dev\Documents\ai-agent-dev\pdfs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E64380A-AA39-4C86-88D9-177E987AF045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="26640" windowHeight="14370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Order Number</t>
   </si>
@@ -37,149 +43,176 @@
     <t>1</t>
   </si>
   <si>
+    <t>23498345933</t>
+  </si>
+  <si>
+    <t>2025 HP Laptop</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
+    <t>23942039482</t>
+  </si>
+  <si>
+    <t>Beanie Baby</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
+    <t>29384023948</t>
+  </si>
+  <si>
+    <t>Collector Pokemon Set</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Christine</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
+    <t>23029849023</t>
+  </si>
+  <si>
+    <t>Dinasaur Pool Toy</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Donna</t>
+  </si>
+  <si>
+    <t>Dorian</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
+    <t>349584398539</t>
+  </si>
+  <si>
+    <t>GoPro</t>
+  </si>
+  <si>
+    <t>$100</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
+    <t>1290138230948</t>
+  </si>
+  <si>
+    <t>inflatable boat</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
+    <t>33945803930</t>
+  </si>
+  <si>
+    <t>stuffed animal bunny</t>
+  </si>
+  <si>
+    <t>$25</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Felicia</t>
+  </si>
+  <si>
     <t>9</t>
   </si>
   <si>
-    <t>23498345933</t>
-  </si>
-  <si>
-    <t>23942039482</t>
-  </si>
-  <si>
-    <t>29384023948</t>
-  </si>
-  <si>
-    <t>23029849023</t>
-  </si>
-  <si>
-    <t>349584398539</t>
-  </si>
-  <si>
-    <t>1290138230948</t>
-  </si>
-  <si>
-    <t>33945803930</t>
-  </si>
-  <si>
     <t>230924802</t>
   </si>
   <si>
-    <t>2025 HP Laptop</t>
-  </si>
-  <si>
-    <t>Beanie Baby</t>
-  </si>
-  <si>
-    <t>Collector Pokemon Set</t>
-  </si>
-  <si>
-    <t>Dinasaur Pool Toy</t>
-  </si>
-  <si>
-    <t>GoPro</t>
-  </si>
-  <si>
-    <t>inflatable boat</t>
-  </si>
-  <si>
-    <t>stuffed animal bunny</t>
-  </si>
-  <si>
     <t>cactus</t>
   </si>
   <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>$100</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>$25</t>
-  </si>
-  <si>
     <t>$300</t>
   </si>
   <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Chad</t>
-  </si>
-  <si>
-    <t>Donna</t>
-  </si>
-  <si>
-    <t>Brian</t>
-  </si>
-  <si>
-    <t>Matt</t>
-  </si>
-  <si>
-    <t>Kelly</t>
-  </si>
-  <si>
     <t>Tim</t>
   </si>
   <si>
-    <t>Aaron</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>Christine</t>
-  </si>
-  <si>
-    <t>Dorian</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Felicia</t>
-  </si>
-  <si>
     <t>Mike</t>
+  </si>
+  <si>
+    <t>$80</t>
+  </si>
+  <si>
+    <t>Mick</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>2320948233</t>
+  </si>
+  <si>
+    <t>box</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>some product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,10 +223,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -242,6 +272,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -529,14 +567,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,167 +599,207 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E9" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
       </c>
       <c r="F9" t="s">
         <v>52</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>23920834209</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OK FINALLY FIXED EXCEL AGENT RAG
</commit_message>
<xml_diff>
--- a/pdfs/order_inventory.xlsx
+++ b/pdfs/order_inventory.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -941,6 +941,390 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Hanna</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Hanna</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>cat</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>dog</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>box</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>circle</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>$2000</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>square</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>square</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>square</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>greg</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>square</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>greg</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>square</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>greg</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2320232342342</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>square</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>greg</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>ian</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
delete function works now
</commit_message>
<xml_diff>
--- a/pdfs/order_inventory.xlsx
+++ b/pdfs/order_inventory.xlsx
@@ -1,102 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric - Dev\Documents\ai-agent-dev\pdfs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC5D7A5-BFAE-48FE-B576-DAAE1A7B14D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26640" windowHeight="14370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Order Number</t>
-  </si>
-  <si>
-    <t>Part Number</t>
-  </si>
-  <si>
-    <t>Order Details</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Seller</t>
-  </si>
-  <si>
-    <t>Buyer</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>23498345933</t>
-  </si>
-  <si>
-    <t>2025 HP Laptop</t>
-  </si>
-  <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>Aaron</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>23942039482</t>
-  </si>
-  <si>
-    <t>Beanie Baby</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -111,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -435,81 +420,145 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Order Number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Order Details</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Seller</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Buyer</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>23498345933</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025 HP Laptop</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>23942039482</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Beanie Baby</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Ben</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>220394820</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>red balloon</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>bob</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>steve</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
txt files and summary of info
</commit_message>
<xml_diff>
--- a/pdfs/order_inventory.xlsx
+++ b/pdfs/order_inventory.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,6 +593,38 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>23402043</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>book</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Fred</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed excel formatting issue
</commit_message>
<xml_diff>
--- a/pdfs/order_inventory.xlsx
+++ b/pdfs/order_inventory.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,6 +625,70 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>order-23</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>23423429</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>car</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>25000</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Jamie</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>24934535</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>box</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12000</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>tom</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>kit</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
bedford plus bot verification implemented and improved
</commit_message>
<xml_diff>
--- a/pdfs/order_inventory.xlsx
+++ b/pdfs/order_inventory.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -689,6 +689,38 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>234343</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>shoe</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>eric</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>meg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>